<commit_message>
Finished task1 subtask 2 for machine learning
</commit_message>
<xml_diff>
--- a/Machine Learning/Task 1/Data/Machine Learning Course At Universities.xlsx
+++ b/Machine Learning/Task 1/Data/Machine Learning Course At Universities.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="79">
   <si>
     <t>University</t>
   </si>
@@ -250,6 +250,9 @@
   </si>
   <si>
     <t>r</t>
+  </si>
+  <si>
+    <t>http://www.cs.columbia.edu/~jebara/4771/notes/class1x.pdf</t>
   </si>
 </sst>
 </file>
@@ -751,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:AH60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C25" workbookViewId="0">
-      <selection activeCell="U60" sqref="U60"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="K52" sqref="K52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1384,7 +1387,10 @@
       <c r="L27" s="6">
         <v>1</v>
       </c>
-      <c r="M27" s="7"/>
+      <c r="M27" s="7">
+        <f t="shared" ref="M27:M47" si="0">SUM(C27:L27)</f>
+        <v>4</v>
+      </c>
       <c r="N27" s="6"/>
       <c r="O27" s="2" t="s">
         <v>14</v>
@@ -1429,13 +1435,16 @@
         <v>1</v>
       </c>
       <c r="L28" s="9"/>
-      <c r="M28" s="10"/>
+      <c r="M28" s="10">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
       <c r="N28" s="9"/>
       <c r="O28" s="3" t="s">
         <v>64</v>
       </c>
       <c r="P28" s="15">
-        <f t="shared" ref="P28:P48" si="0">SUM(Q28:U28)</f>
+        <f t="shared" ref="P28:P48" si="1">SUM(Q28:U28)</f>
         <v>0</v>
       </c>
       <c r="Q28" s="9"/>
@@ -1460,13 +1469,16 @@
       <c r="J29" s="9"/>
       <c r="K29" s="9"/>
       <c r="L29" s="9"/>
-      <c r="M29" s="10"/>
+      <c r="M29" s="10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="N29" s="9"/>
       <c r="O29" s="3" t="s">
         <v>26</v>
       </c>
       <c r="P29" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q29" s="9"/>
@@ -1491,13 +1503,16 @@
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
       <c r="L30" s="9"/>
-      <c r="M30" s="10"/>
+      <c r="M30" s="10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="N30" s="9"/>
       <c r="O30" s="3" t="s">
         <v>15</v>
       </c>
       <c r="P30" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q30" s="9"/>
@@ -1532,13 +1547,16 @@
       <c r="L31" s="9">
         <v>1</v>
       </c>
-      <c r="M31" s="10"/>
+      <c r="M31" s="10">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
       <c r="N31" s="9"/>
       <c r="O31" s="3" t="s">
         <v>25</v>
       </c>
       <c r="P31" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="Q31" s="9">
@@ -1569,13 +1587,16 @@
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
       <c r="L32" s="9"/>
-      <c r="M32" s="10"/>
+      <c r="M32" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="N32" s="9"/>
       <c r="O32" s="3" t="s">
         <v>27</v>
       </c>
       <c r="P32" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q32" s="9"/>
@@ -1612,13 +1633,16 @@
       <c r="L33" s="9">
         <v>1</v>
       </c>
-      <c r="M33" s="10"/>
+      <c r="M33" s="10">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
       <c r="N33" s="9"/>
       <c r="O33" s="3" t="s">
         <v>48</v>
       </c>
       <c r="P33" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="Q33" s="9">
@@ -1671,13 +1695,16 @@
       <c r="L34" s="9">
         <v>1</v>
       </c>
-      <c r="M34" s="10"/>
+      <c r="M34" s="10">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="N34" s="9"/>
       <c r="O34" s="3" t="s">
         <v>2</v>
       </c>
       <c r="P34" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="Q34" s="9"/>
@@ -1720,13 +1747,16 @@
         <v>1</v>
       </c>
       <c r="L35" s="9"/>
-      <c r="M35" s="10"/>
+      <c r="M35" s="10">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
       <c r="N35" s="9"/>
       <c r="O35" s="3" t="s">
         <v>5</v>
       </c>
       <c r="P35" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="Q35" s="9"/>
@@ -1759,13 +1789,16 @@
         <v>1</v>
       </c>
       <c r="L36" s="9"/>
-      <c r="M36" s="10"/>
+      <c r="M36" s="10">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
       <c r="N36" s="9"/>
       <c r="O36" s="3" t="s">
         <v>6</v>
       </c>
       <c r="P36" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="Q36" s="9">
@@ -1794,13 +1827,16 @@
       <c r="J37" s="9"/>
       <c r="K37" s="9"/>
       <c r="L37" s="9"/>
-      <c r="M37" s="10"/>
+      <c r="M37" s="10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="N37" s="9"/>
       <c r="O37" s="3" t="s">
         <v>7</v>
       </c>
       <c r="P37" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q37" s="9"/>
@@ -1827,13 +1863,16 @@
       <c r="J38" s="9"/>
       <c r="K38" s="9"/>
       <c r="L38" s="9"/>
-      <c r="M38" s="10"/>
+      <c r="M38" s="10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
       <c r="N38" s="9"/>
       <c r="O38" s="3" t="s">
         <v>8</v>
       </c>
       <c r="P38" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q38" s="9"/>
@@ -1862,13 +1901,16 @@
       <c r="L39" s="9">
         <v>1</v>
       </c>
-      <c r="M39" s="10"/>
+      <c r="M39" s="10">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
       <c r="N39" s="9"/>
       <c r="O39" s="3" t="s">
         <v>21</v>
       </c>
       <c r="P39" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Q39" s="9"/>
@@ -1901,13 +1943,16 @@
       <c r="L40" s="9">
         <v>1</v>
       </c>
-      <c r="M40" s="10"/>
+      <c r="M40" s="10">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
       <c r="N40" s="9"/>
       <c r="O40" s="3" t="s">
         <v>12</v>
       </c>
       <c r="P40" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="Q40" s="9"/>
@@ -1944,13 +1989,16 @@
         <v>1</v>
       </c>
       <c r="L41" s="9"/>
-      <c r="M41" s="10"/>
+      <c r="M41" s="10">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
       <c r="N41" s="9"/>
       <c r="O41" s="3" t="s">
         <v>65</v>
       </c>
       <c r="P41" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q41" s="9"/>
@@ -1981,13 +2029,16 @@
       </c>
       <c r="K42" s="9"/>
       <c r="L42" s="9"/>
-      <c r="M42" s="10"/>
+      <c r="M42" s="10">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
       <c r="N42" s="9"/>
       <c r="O42" s="3" t="s">
         <v>63</v>
       </c>
       <c r="P42" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Q42" s="9">
@@ -2022,13 +2073,16 @@
         <v>1</v>
       </c>
       <c r="L43" s="9"/>
-      <c r="M43" s="10"/>
+      <c r="M43" s="10">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
       <c r="N43" s="9"/>
       <c r="O43" s="3" t="s">
         <v>13</v>
       </c>
       <c r="P43" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="Q43" s="9"/>
@@ -2059,13 +2113,16 @@
       <c r="J44" s="9"/>
       <c r="K44" s="9"/>
       <c r="L44" s="9"/>
-      <c r="M44" s="10"/>
+      <c r="M44" s="10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="N44" s="9"/>
       <c r="O44" s="3" t="s">
         <v>66</v>
       </c>
       <c r="P44" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q44" s="9"/>
@@ -2096,13 +2153,16 @@
         <v>1</v>
       </c>
       <c r="L45" s="9"/>
-      <c r="M45" s="10"/>
+      <c r="M45" s="10">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
       <c r="N45" s="9"/>
       <c r="O45" s="3" t="s">
         <v>19</v>
       </c>
       <c r="P45" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Q45" s="9"/>
@@ -2127,13 +2187,16 @@
       <c r="J46" s="9"/>
       <c r="K46" s="9"/>
       <c r="L46" s="9"/>
-      <c r="M46" s="10"/>
+      <c r="M46" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="N46" s="9"/>
       <c r="O46" s="3" t="s">
         <v>56</v>
       </c>
       <c r="P46" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Q46" s="9"/>
@@ -2168,13 +2231,16 @@
       <c r="J47" s="9"/>
       <c r="K47" s="9"/>
       <c r="L47" s="9"/>
-      <c r="M47" s="10"/>
+      <c r="M47" s="10">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
       <c r="N47" s="9"/>
       <c r="O47" s="3" t="s">
         <v>21</v>
       </c>
       <c r="P47" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="Q47" s="9">
@@ -2207,13 +2273,16 @@
       <c r="J48" s="12"/>
       <c r="K48" s="12"/>
       <c r="L48" s="12"/>
-      <c r="M48" s="13"/>
+      <c r="M48" s="13">
+        <f>SUM(C48:L48)</f>
+        <v>1</v>
+      </c>
       <c r="N48" s="12"/>
       <c r="O48" s="4" t="s">
         <v>28</v>
       </c>
       <c r="P48" s="16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q48" s="12"/>
@@ -2284,6 +2353,9 @@
       </c>
       <c r="J50" s="1" t="s">
         <v>70</v>
+      </c>
+      <c r="K50" t="s">
+        <v>78</v>
       </c>
       <c r="L50" t="s">
         <v>40</v>
@@ -2354,9 +2426,11 @@
     <hyperlink ref="R60" r:id="rId7"/>
     <hyperlink ref="Q60" r:id="rId8"/>
     <hyperlink ref="T60" r:id="rId9"/>
+    <hyperlink ref="I50" r:id="rId10"/>
+    <hyperlink ref="J50" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId10"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId12"/>
 </worksheet>
 </file>
 

</xml_diff>